<commit_message>
di excel, ubah link website
</commit_message>
<xml_diff>
--- a/kerjaan/untag/nota kelola web untag.xlsx
+++ b/kerjaan/untag/nota kelola web untag.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\zen\kerjaan\untag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCB87BF-B6B9-4076-8901-C73C794B1908}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6D9293-BB1A-45FF-BCCD-D441768DD421}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{39030E98-4251-4D69-AD84-027202D63649}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Jasa Pengolahan Website</t>
   </si>
   <si>
-    <t>WA: 0815 4514 3654 | website: jasazen.my.id</t>
-  </si>
-  <si>
     <t>Layanan</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>24 Juli 2023</t>
+  </si>
+  <si>
+    <t>WA: 0815 4514 3654 | website: zen.mabaiz.web.id</t>
   </si>
 </sst>
 </file>
@@ -236,16 +236,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -565,7 +565,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,58 +580,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="A2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="I4" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4">
         <v>10000</v>
@@ -640,14 +640,14 @@
         <v>50</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:E10" si="0">B5*C5</f>
         <v>500000</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="5">
         <v>1000000</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4">
         <v>10000</v>
@@ -668,14 +668,14 @@
         <v>580</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>5800000</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="5">
         <v>1000000</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4">
         <v>150000</v>
@@ -696,7 +696,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
@@ -705,7 +705,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4">
         <v>150000</v>
@@ -714,7 +714,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
@@ -723,7 +723,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4">
         <v>150000</v>
@@ -732,7 +732,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
@@ -741,7 +741,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="7">
         <v>150000</v>
@@ -750,7 +750,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="0"/>
@@ -762,7 +762,7 @@
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="13">
         <f>SUM(E5:E10)</f>

</xml_diff>